<commit_message>
Update 04 Desember 2023 - Change email to username login function - Fitur Import
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_LOG_FINGER_NEW.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_LOG_FINGER_NEW.xlsx
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
   <si>
-    <t xml:space="preserve">LOG_AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN_OUT</t>
-  </si>
-  <si>
     <t xml:space="preserve">CODE_SN_FINGER</t>
   </si>
   <si>
@@ -43,23 +37,25 @@
     <t xml:space="preserve">CODE_PIN</t>
   </si>
   <si>
-    <t xml:space="preserve">0323230002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0323230003</t>
+    <t xml:space="preserve">TIME_IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME_OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANGGAL_LOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABSEN_TYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -94,8 +90,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -140,15 +136,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,48 +149,12 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -213,7 +169,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFE7E6E6"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -226,7 +182,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -278,89 +234,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.7734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="3" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="27.72"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="11" t="n">
-        <v>45231.3263888889</v>
-      </c>
-      <c r="C2" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="11" t="n">
-        <v>45231.3263888889</v>
-      </c>
-      <c r="F2" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8" t="n">
-        <v>111</v>
-      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="11" t="n">
-        <v>45231.3263888889</v>
-      </c>
-      <c r="C3" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="11" t="n">
-        <v>45231.3263888889</v>
-      </c>
-      <c r="F3" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>222</v>
-      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0"/>

</xml_diff>

<commit_message>
Update 22 January 2024 - Import Shift Schedule - Create Overtime, Leave, Tukar Shift Mobile
</commit_message>
<xml_diff>
--- a/public/template_import/TEMPLATE_IMPORT_LOG_FINGER_NEW.xlsx
+++ b/public/template_import/TEMPLATE_IMPORT_LOG_FINGER_NEW.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">KD_PGW</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">ABSEN_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-01 07:50:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-01 05:05:00</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,6 +161,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -236,16 +246,16 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.7890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.79296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="27.72"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,10 +288,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
+      <c r="A2" s="0" t="n">
+        <v>323230002</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="0"/>

</xml_diff>